<commit_message>
CHANGE: Remove empty cells
</commit_message>
<xml_diff>
--- a/data/modified/charities_sizes.xlsx
+++ b/data/modified/charities_sizes.xlsx
@@ -3343,10 +3343,13 @@
       <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
+    </dxf>
+    <dxf>
       <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="0.000000"/>
+      <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.000000"/>
@@ -3358,10 +3361,7 @@
       <numFmt numFmtId="3" formatCode="#,##0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="3" formatCode="#,##0"/>
+      <numFmt numFmtId="164" formatCode="0.000000"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="3" formatCode="#,##0"/>
@@ -3403,25 +3403,25 @@
     <tableColumn id="48" xr3:uid="{00000000-0010-0000-0000-000030000000}" name="revenue" dataDxfId="8">
       <calculatedColumnFormula>Table1[[#This Row],[receipts_total]]-Table1[[#This Row],[receipts_others_income]]</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="1" xr3:uid="{925E8B84-6631-2E40-A6CE-C701F593A881}" name="revenue_log" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{925E8B84-6631-2E40-A6CE-C701F593A881}" name="revenue_log" dataDxfId="7">
       <calculatedColumnFormula>LOG(Table1[[#This Row],[revenue]]+1,10)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="charity_size" dataDxfId="7">
+    <tableColumn id="49" xr3:uid="{00000000-0010-0000-0000-000031000000}" name="charity_size" dataDxfId="6">
       <calculatedColumnFormula>IF(Table1[[#This Row],[revenue]]&lt;250000,"S",IF(Table1[[#This Row],[revenue]]&lt;1000000,"M","L"))</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="charity_size_small" dataDxfId="6">
+    <tableColumn id="50" xr3:uid="{00000000-0010-0000-0000-000032000000}" name="charity_size_small" dataDxfId="5">
       <calculatedColumnFormula>IF(Table1[[#This Row],[charity_size]]="S",1, 0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="charity_size_small_cf" dataDxfId="3">
+    <tableColumn id="53" xr3:uid="{00000000-0010-0000-0000-000035000000}" name="charity_size_small_cf" dataDxfId="4">
       <calculatedColumnFormula>IF(Table1[[#This Row],[charity_size]]="S",(Table1[[#This Row],[revenue_log]]-_xlfn.MINIFS($J$2:$J$423,$K$2:$K$423,"S"))/(_xlfn.MAXIFS($J$2:$J$423,$K$2:$K$423,"S")-_xlfn.MINIFS($J$2:$J$423,$K$2:$K$423,"S")),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="charity_size_medium" dataDxfId="5">
+    <tableColumn id="51" xr3:uid="{00000000-0010-0000-0000-000033000000}" name="charity_size_medium" dataDxfId="3">
       <calculatedColumnFormula>IF(Table1[[#This Row],[charity_size]]="M",1,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="54" xr3:uid="{00000000-0010-0000-0000-000036000000}" name="charity_size_medium_cf" dataDxfId="2">
       <calculatedColumnFormula>IF(Table1[[#This Row],[charity_size]]="M",(Table1[[#This Row],[revenue_log]]-_xlfn.MINIFS($J$2:$J$423,$K$2:$K$423,"M"))/(_xlfn.MAXIFS($J$2:$J$423,$K$2:$K$423,"M")-_xlfn.MINIFS($J$2:$J$423,$K$2:$K$423,"M")),0)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="charity_size_large" dataDxfId="4">
+    <tableColumn id="52" xr3:uid="{00000000-0010-0000-0000-000034000000}" name="charity_size_large" dataDxfId="1">
       <calculatedColumnFormula>IF(Table1[[#This Row],[charity_size]]="L",1,0)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="55" xr3:uid="{00000000-0010-0000-0000-000037000000}" name="charity_size_large_cf" dataDxfId="0">
@@ -3729,10 +3729,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:V451"/>
+  <dimension ref="A1:Q451"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I212" workbookViewId="0">
-      <selection activeCell="Q227" sqref="Q227"/>
+    <sheetView tabSelected="1" topLeftCell="M65" workbookViewId="0">
+      <selection activeCell="R65" sqref="R1:W1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3753,16 +3753,14 @@
     <col min="15" max="15" width="24.1640625" style="2" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="18.83203125" bestFit="1" customWidth="1"/>
     <col min="17" max="17" width="21.33203125" style="2" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.83203125" customWidth="1"/>
-    <col min="23" max="23" width="34.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="37.83203125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="41" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="23.1640625" customWidth="1"/>
-    <col min="42" max="42" width="25.1640625" customWidth="1"/>
-    <col min="43" max="43" width="14.83203125" customWidth="1"/>
+    <col min="18" max="18" width="37.83203125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="41" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="23.1640625" customWidth="1"/>
+    <col min="36" max="36" width="25.1640625" customWidth="1"/>
+    <col min="37" max="37" width="14.83203125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:17" x14ac:dyDescent="0.2">
@@ -7724,7 +7722,7 @@
         <v>0.3124415891482763</v>
       </c>
     </row>
-    <row r="65" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
         <v>358</v>
       </c>
@@ -7786,7 +7784,7 @@
         <v>0.30296126182527816</v>
       </c>
     </row>
-    <row r="66" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
         <v>399</v>
       </c>
@@ -7848,7 +7846,7 @@
         <v>0.30288108864309965</v>
       </c>
     </row>
-    <row r="67" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
         <v>492</v>
       </c>
@@ -7910,7 +7908,7 @@
         <v>0.29827552979681182</v>
       </c>
     </row>
-    <row r="68" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
         <v>586</v>
       </c>
@@ -7972,7 +7970,7 @@
         <v>0.29704882644920477</v>
       </c>
     </row>
-    <row r="69" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
         <v>507</v>
       </c>
@@ -8034,7 +8032,7 @@
         <v>0.29639290903248661</v>
       </c>
     </row>
-    <row r="70" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
         <v>515</v>
       </c>
@@ -8095,12 +8093,8 @@
         <f>IF(Table1[[#This Row],[charity_size]]="L",(Table1[[#This Row],[revenue_log]]-_xlfn.MINIFS($J$2:$J$423,$K$2:$K$423,"L"))/(_xlfn.MAXIFS($J$2:$J$423,$K$2:$K$423,"L")-_xlfn.MINIFS($J$2:$J$423,$K$2:$K$423,"L")),0)</f>
         <v>0.29281343145657301</v>
       </c>
-      <c r="V70">
-        <f>LOG10(1)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="1:22" x14ac:dyDescent="0.2">
+    </row>
+    <row r="71" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
         <v>811</v>
       </c>
@@ -8162,7 +8156,7 @@
         <v>0.29197036934302939</v>
       </c>
     </row>
-    <row r="72" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
         <v>439</v>
       </c>
@@ -8224,7 +8218,7 @@
         <v>0.28819351653838687</v>
       </c>
     </row>
-    <row r="73" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
         <v>505</v>
       </c>
@@ -8286,7 +8280,7 @@
         <v>0.28634661422332219</v>
       </c>
     </row>
-    <row r="74" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
         <v>75</v>
       </c>
@@ -8348,7 +8342,7 @@
         <v>0.2846403644032538</v>
       </c>
     </row>
-    <row r="75" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
         <v>474</v>
       </c>
@@ -8410,7 +8404,7 @@
         <v>0.2832287945827931</v>
       </c>
     </row>
-    <row r="76" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
         <v>374</v>
       </c>
@@ -8472,7 +8466,7 @@
         <v>0.28245892694562308</v>
       </c>
     </row>
-    <row r="77" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
         <v>673</v>
       </c>
@@ -8534,7 +8528,7 @@
         <v>0.2820029525453312</v>
       </c>
     </row>
-    <row r="78" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
         <v>638</v>
       </c>
@@ -8596,7 +8590,7 @@
         <v>0.27404341786472247</v>
       </c>
     </row>
-    <row r="79" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
         <v>519</v>
       </c>
@@ -8658,7 +8652,7 @@
         <v>0.27380973353573895</v>
       </c>
     </row>
-    <row r="80" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
         <v>797</v>
       </c>

</xml_diff>